<commit_message>
Fiz a funão de visualizar as atividades pendentes
</commit_message>
<xml_diff>
--- a/Fluxo Caixa Construção Guaratinguetá.xlsx
+++ b/Fluxo Caixa Construção Guaratinguetá.xlsx
@@ -56,7 +56,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -127,6 +127,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF57BB8A"/>
         <bgColor rgb="FF57BB8A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0092D050"/>
+        <bgColor rgb="0092D050"/>
       </patternFill>
     </fill>
   </fills>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -227,12 +233,8 @@
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -248,9 +250,7 @@
     <xf numFmtId="165" fontId="5" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -266,9 +266,7 @@
     <xf numFmtId="165" fontId="6" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -278,36 +276,28 @@
     <xf numFmtId="164" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -399,9 +389,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -414,6 +402,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,7 +805,7 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="15.13" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="15.13" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col width="16.38" customWidth="1" style="72" min="1" max="1"/>
     <col width="14.5" customWidth="1" style="72" min="2" max="2"/>
@@ -1023,27 +1021,33 @@
       <c r="G11" s="71" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="36" t="n">
+      <c r="A12" s="79" t="n">
         <v>44160</v>
       </c>
-      <c r="B12" s="11" t="n">
+      <c r="B12" s="80" t="n">
         <v>3900</v>
       </c>
-      <c r="C12" s="70" t="inlineStr">
+      <c r="C12" s="81" t="inlineStr">
         <is>
           <t>Caixa Economica</t>
         </is>
       </c>
-      <c r="D12" s="70" t="inlineStr">
+      <c r="D12" s="81" t="inlineStr">
         <is>
           <t>Parcela de Financiamento Casa</t>
         </is>
       </c>
-      <c r="E12" s="11" t="n">
+      <c r="E12" s="80" t="n">
         <v>3900</v>
       </c>
-      <c r="F12" s="11" t="n"/>
-      <c r="G12" s="71" t="n"/>
+      <c r="F12" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="71" t="inlineStr">
+        <is>
+          <t>14/04/2025</t>
+        </is>
+      </c>
     </row>
     <row r="13" collapsed="1" s="72">
       <c r="A13" s="36" t="n">
@@ -7942,23 +7946,29 @@
       <c r="G325" s="71" t="n"/>
     </row>
     <row r="326">
-      <c r="A326" s="36" t="n"/>
-      <c r="B326" s="21" t="n">
+      <c r="A326" s="79" t="n"/>
+      <c r="B326" s="80" t="n">
         <v>1000</v>
       </c>
-      <c r="C326" s="71" t="inlineStr">
+      <c r="C326" s="82" t="inlineStr">
         <is>
           <t>EDP</t>
         </is>
       </c>
-      <c r="D326" s="71" t="inlineStr">
+      <c r="D326" s="82" t="inlineStr">
         <is>
           <t>Conta de Energia 2025</t>
         </is>
       </c>
-      <c r="E326" s="21" t="n"/>
-      <c r="F326" s="21" t="n"/>
-      <c r="G326" s="71" t="n"/>
+      <c r="E326" s="80" t="n"/>
+      <c r="F326" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G326" s="71" t="inlineStr">
+        <is>
+          <t>14/04/2025</t>
+        </is>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="28" t="n"/>
@@ -8039,23 +8049,29 @@
       <c r="G330" s="71" t="n"/>
     </row>
     <row r="331">
-      <c r="A331" s="36" t="n"/>
-      <c r="B331" s="21" t="n">
+      <c r="A331" s="79" t="n"/>
+      <c r="B331" s="80" t="n">
         <v>1000</v>
       </c>
-      <c r="C331" s="71" t="inlineStr">
+      <c r="C331" s="82" t="inlineStr">
         <is>
           <t>SAEG</t>
         </is>
       </c>
-      <c r="D331" s="71" t="inlineStr">
+      <c r="D331" s="82" t="inlineStr">
         <is>
           <t>Conta de Água 2025</t>
         </is>
       </c>
-      <c r="E331" s="21" t="n"/>
-      <c r="F331" s="21" t="n"/>
-      <c r="G331" s="71" t="n"/>
+      <c r="E331" s="80" t="n"/>
+      <c r="F331" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G331" s="71" t="inlineStr">
+        <is>
+          <t>14/04/2025</t>
+        </is>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="28" t="n"/>

</xml_diff>

<commit_message>
Adcionei o modal para visualizar as informações
</commit_message>
<xml_diff>
--- a/Fluxo Caixa Construção Guaratinguetá.xlsx
+++ b/Fluxo Caixa Construção Guaratinguetá.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpbit\Documents\Projeto Obra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FE2A97-1FAD-43B0-98B0-342218957625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95660A75-493C-40E6-A7A6-134AC8978A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="2445" windowWidth="16305" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Despesas" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="207">
   <si>
     <t>GASTOS  COM A OBRA DA CASA DE GUARATINGUETÁ</t>
   </si>
@@ -1065,6 +1065,10 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1073,10 +1077,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,9 +1384,9 @@
   </sheetPr>
   <dimension ref="A1:I1222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1400,23 +1400,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="66"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1585,9 +1585,7 @@
       <c r="F12" s="58">
         <v>1</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
@@ -3158,7 +3156,7 @@
       <c r="F92" s="5">
         <v>950</v>
       </c>
-      <c r="G92" s="67"/>
+      <c r="G92" s="61"/>
     </row>
     <row r="93" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="19"/>
@@ -3225,7 +3223,7 @@
       </c>
       <c r="F96" s="8"/>
       <c r="G96" s="9"/>
-      <c r="I96" s="68"/>
+      <c r="I96" s="62"/>
     </row>
     <row r="97" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="4">

</xml_diff>